<commit_message>
Commit ECR and BEP(ECR is still unstable)
</commit_message>
<xml_diff>
--- a/Data Files/ECR/TestDataECR.xlsx
+++ b/Data Files/ECR/TestDataECR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAUIAutomation\Data Files\ECR\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
   <si>
     <t>pogoa@pegasystems.com</t>
   </si>
@@ -74,9 +74,6 @@
     <t>lachd@pegasystems.com</t>
   </si>
   <si>
-    <t>diets@pegasystems.com</t>
-  </si>
-  <si>
     <t>FFTHRDBANK</t>
   </si>
   <si>
@@ -110,21 +107,6 @@
     <t>\Data Files\ECR\PCR_3.xlsm</t>
   </si>
   <si>
-    <t>ECR-01Apr2018-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR-28Mar2018-24
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR-29Mar2018-7
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR-29Mar2018-1
-</t>
-  </si>
-  <si>
     <t>CR</t>
   </si>
   <si>
@@ -134,52 +116,63 @@
     <t>PROJ ID</t>
   </si>
   <si>
-    <t>P001787</t>
-  </si>
-  <si>
-    <t>P001788</t>
-  </si>
-  <si>
-    <t>P001788-001</t>
-  </si>
-  <si>
-    <t>CR-44465</t>
-  </si>
-  <si>
-    <t>P001787-002</t>
-  </si>
-  <si>
-    <t>CR-44466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR-03Nov2017-6
-</t>
+    <t>PegaServiceValue</t>
+  </si>
+  <si>
+    <t>ECR-25Apr2018-12</t>
+  </si>
+  <si>
+    <t>ECR-25Apr2018-13</t>
+  </si>
+  <si>
+    <t>ECR-25Apr2018-14</t>
+  </si>
+  <si>
+    <t>ECR-25Apr2018-15</t>
+  </si>
+  <si>
+    <t>ECR-25Apr2018-16</t>
+  </si>
+  <si>
+    <t>martw@pegasystems.com</t>
+  </si>
+  <si>
+    <t>ECR-03May2018-9</t>
+  </si>
+  <si>
+    <t>ECR-09Apr2018-19</t>
   </si>
   <si>
     <t>marsa@pegasystems.com</t>
   </si>
   <si>
-    <t>waink@pegasystems.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR-07Apr2018-2
-</t>
-  </si>
-  <si>
-    <t>P001791</t>
-  </si>
-  <si>
-    <t>P001791-002</t>
-  </si>
-  <si>
-    <t>CR-44468</t>
+    <t>ECR-03Jul2018-5</t>
+  </si>
+  <si>
+    <t>ECR-03Jul2018-7</t>
+  </si>
+  <si>
+    <t>ECR-03Jul2018-8</t>
+  </si>
+  <si>
+    <t>ECR-06Jul2018-1</t>
+  </si>
+  <si>
+    <t>ECR-06Jul2018-5</t>
+  </si>
+  <si>
+    <t>ECR-09Jul2018-4</t>
+  </si>
+  <si>
+    <t>ECR-09Jul2018-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,31 +586,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="17.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="11" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="3" max="6" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -625,387 +616,376 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>4</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>4</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>4</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>4</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>4</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId4"/>
+    <hyperlink ref="K2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>